<commit_message>
update confronto prestazioni con shared memory in kernel righe
</commit_message>
<xml_diff>
--- a/test versioni/Confronto prestazioni.xlsx
+++ b/test versioni/Confronto prestazioni.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E205E550-A030-42D5-A6EE-8FF3343D96C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C6562B-72DC-4324-98B5-D0510E0C7C94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Versione 1</t>
   </si>
@@ -92,6 +92,12 @@
   <si>
     <t>CPU-Righe ratio</t>
   </si>
+  <si>
+    <t>shared</t>
+  </si>
+  <si>
+    <t>CPU-shared ratio</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +106,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.0000_ ;\-0.0000\ "/>
+    <numFmt numFmtId="165" formatCode="0.0000_ ;\-0.0000\ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -143,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -1152,6 +1158,470 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Confronto</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> kernel</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$C$8:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.907</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.473000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.335000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>431.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>479.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>842.13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>930.20600000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0634-4A2F-9165-E0BCDEC09923}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$C$28:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.8959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8310000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.605</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.404000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>290.44900000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>327.10300000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>536.72500000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>610.55600000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0634-4A2F-9165-E0BCDEC09923}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$D$28:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.7929999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4560000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.468000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>270.30500000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>302.471</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>503.774</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>572.81399999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0634-4A2F-9165-E0BCDEC09923}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="306928000"/>
+        <c:axId val="306928656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="306928000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="306928656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="306928656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="306928000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1232,6 +1702,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1749,6 +2259,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2333,6 +3359,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87ECFCF2-AA93-4164-A72E-1BF68CAFD078}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2604,10 +3666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,7 +3678,7 @@
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2974,8 +4036,313 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="C17" s="2">
+        <v>930.20600000000002</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
+        <v>6.6906999999999994E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.034</v>
+      </c>
+      <c r="E22" s="2">
+        <f>B22/D22</f>
+        <v>6.4706963249516428E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2">
+        <v>8.3939E-2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" ref="E23:E37" si="2">B23/D23</f>
+        <v>0.28648122866894199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.29321999999999998</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.432</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="2"/>
+        <v>0.67874999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4.9819000000000002E-2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="2"/>
+        <v>0.17985198555956677</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.64874299999999996</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2036048237476806</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.34740300000000002</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.438</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="2"/>
+        <v>0.79315753424657542</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="3">
+        <v>6.0758000000000001</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.8959999999999999</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.7929999999999999</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="2"/>
+        <v>3.388622420524261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2">
+        <v>3.1732</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.468</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.3520000000000001</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="2"/>
+        <v>2.3470414201183432</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2">
+        <v>52.365499999999997</v>
+      </c>
+      <c r="C30" s="2">
+        <v>11.436</v>
+      </c>
+      <c r="D30" s="2">
+        <v>10.568</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="2"/>
+        <v>4.9551003028009086</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2">
+        <v>17.5593</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4.8310000000000004</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4.4560000000000004</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="2"/>
+        <v>3.9405969479353677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2">
+        <v>169.84</v>
+      </c>
+      <c r="C32" s="2">
+        <v>31.605</v>
+      </c>
+      <c r="D32" s="2">
+        <v>29.529</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="2"/>
+        <v>5.7516339869281046</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="2">
+        <v>303.58</v>
+      </c>
+      <c r="C33" s="2">
+        <v>50.404000000000003</v>
+      </c>
+      <c r="D33" s="2">
+        <v>46.468000000000004</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="2"/>
+        <v>6.5330980459671162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2086.73</v>
+      </c>
+      <c r="C34" s="2">
+        <v>290.44900000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>270.30500000000001</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="2"/>
+        <v>7.7199089916945667</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2292.75</v>
+      </c>
+      <c r="C35" s="2">
+        <v>327.10300000000001</v>
+      </c>
+      <c r="D35" s="2">
+        <v>302.471</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="2"/>
+        <v>7.5800655269430788</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="2">
+        <v>4083.51</v>
+      </c>
+      <c r="C36" s="2">
+        <v>536.72500000000002</v>
+      </c>
+      <c r="D36" s="2">
+        <v>503.774</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="2"/>
+        <v>8.105837141257787</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="2">
+        <v>610.55600000000004</v>
+      </c>
+      <c r="D37" s="2">
+        <v>572.81399999999996</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
clean file e test blocco ottimizzato
</commit_message>
<xml_diff>
--- a/test versioni/Confronto prestazioni.xlsx
+++ b/test versioni/Confronto prestazioni.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E2DA2E-F223-4856-B6B6-9692A03CE967}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BAF8CA-E327-431E-99B2-2FC7749218CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
   <si>
     <t>Versione 1</t>
   </si>
@@ -125,6 +125,12 @@
   <si>
     <t>blocco-cpu</t>
   </si>
+  <si>
+    <t>blocco-cpu optimazed</t>
+  </si>
+  <si>
+    <t>blocco-o</t>
+  </si>
 </sst>
 </file>
 
@@ -180,13 +186,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -2610,16 +2617,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1066799</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2646,16 +2653,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2948,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2965,7 @@
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3724,7 +3731,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -3741,7 +3748,7 @@
         <v>0.47899999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -3758,7 +3765,7 @@
         <v>1.724</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -3775,7 +3782,7 @@
         <v>1.323</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -3792,7 +3799,7 @@
         <v>8.2759999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -3809,7 +3816,7 @@
         <v>3.7749999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -3826,7 +3833,7 @@
         <v>21.007999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -3843,7 +3850,7 @@
         <v>34.087000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -3860,7 +3867,7 @@
         <v>185.351</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -3877,7 +3884,7 @@
         <v>209.85900000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3894,7 +3901,7 @@
         <v>341.274</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3908,10 +3915,10 @@
         <v>387.42500000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E60" s="4"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -3927,8 +3934,11 @@
       <c r="E62" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -3944,8 +3954,11 @@
       <c r="E63" s="2">
         <v>3.7749999999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="2">
+        <v>2.028</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -3961,8 +3974,11 @@
       <c r="E64" s="2">
         <v>8.2759999999999998</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="2">
+        <v>4.3079999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -3978,8 +3994,11 @@
       <c r="E65" s="2">
         <v>21.007999999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="2">
+        <v>10.448</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -3995,8 +4014,11 @@
       <c r="E66" s="5">
         <v>34.087000000000003</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="2">
+        <v>18.902000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -4012,8 +4034,11 @@
       <c r="E67" s="2">
         <v>185.351</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>124.38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -4029,8 +4054,11 @@
       <c r="E68" s="2">
         <v>209.85900000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="2">
+        <v>135.93199999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -4046,8 +4074,11 @@
       <c r="E69" s="2">
         <v>341.274</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="2">
+        <v>248.55699999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -4060,8 +4091,11 @@
       <c r="E70" s="2">
         <v>387.42500000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="6">
+        <v>268.56799999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>29</v>
       </c>
@@ -4074,8 +4108,11 @@
       <c r="D78" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -4091,123 +4128,155 @@
         <f>B63/E63</f>
         <v>4.6514701986754972</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="2">
+        <f t="shared" ref="E79:E80" si="3">B63/F63</f>
+        <v>8.6584319526627223</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="2">
-        <f t="shared" ref="B80:B86" si="3">B64/C64</f>
+        <f t="shared" ref="B80:B86" si="4">B64/C64</f>
         <v>4.1983083460274191</v>
       </c>
       <c r="C80" s="2">
-        <f t="shared" ref="C80:C86" si="4">B64/D64</f>
+        <f t="shared" ref="C80:C86" si="5">B64/D64</f>
         <v>4.9551003028009086</v>
       </c>
       <c r="D80" s="2">
-        <f t="shared" ref="D80:D86" si="5">B64/E64</f>
+        <f t="shared" ref="D80:D86" si="6">B64/E64</f>
         <v>6.3273924601256644</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="2">
+        <f t="shared" si="3"/>
+        <v>12.155408542246983</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>10</v>
       </c>
       <c r="B81" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.8065657280316962</v>
       </c>
       <c r="C81" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.7516339869281046</v>
       </c>
       <c r="D81" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.0845392231530848</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="2">
+        <f>B65/F65</f>
+        <v>16.255742725880552</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>11</v>
       </c>
       <c r="B82" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.5514242878560713</v>
       </c>
       <c r="C82" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.5330980459671162</v>
       </c>
       <c r="D82" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.9060345586293881</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="2">
+        <f t="shared" ref="E82:E86" si="7">B66/F66</f>
+        <v>16.060734313829222</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
       <c r="B83" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.8378967379964299</v>
       </c>
       <c r="C83" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.7199089916945667</v>
       </c>
       <c r="D83" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.258261352784716</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="2">
+        <f t="shared" si="7"/>
+        <v>16.777054188776333</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>13</v>
       </c>
       <c r="B84" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.7811444300788253</v>
       </c>
       <c r="C84" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.5800655269430788</v>
       </c>
       <c r="D84" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10.92519262933684</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="2">
+        <f t="shared" si="7"/>
+        <v>16.866889327016452</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>14</v>
       </c>
       <c r="B85" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.8490256848705071</v>
       </c>
       <c r="C85" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.105837141257787</v>
       </c>
       <c r="D85" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.965488141493346</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="2">
+        <f t="shared" si="7"/>
+        <v>16.428867422764196</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>15</v>
       </c>
       <c r="B86" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C86" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="C86" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="D86" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E86" s="2">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
aggiunto progetto visual studio
</commit_message>
<xml_diff>
--- a/test versioni/Confronto prestazioni.xlsx
+++ b/test versioni/Confronto prestazioni.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BAF8CA-E327-431E-99B2-2FC7749218CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BAF8CA-E327-431E-99B2-2FC7749218CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>

</xml_diff>